<commit_message>
add plots for databalancing
</commit_message>
<xml_diff>
--- a/RagaList.xlsx
+++ b/RagaList.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhythmjain/GT-files/2-2/CompMus/ComputationalMusicology-TheRagaGuide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E86B788-15BE-D64D-8BBF-125778262870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4A00FB-CC9E-5647-8017-5325E8ACF4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$75</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="185">
   <si>
     <t>Raga</t>
   </si>
@@ -140,9 +143,6 @@
     <t xml:space="preserve">Ga </t>
   </si>
   <si>
-    <t>Na</t>
-  </si>
-  <si>
     <t>Bilaskhani Todi</t>
   </si>
   <si>
@@ -573,6 +573,24 @@
   </si>
   <si>
     <t>ramkali.txt</t>
+  </si>
+  <si>
+    <t>ALT_Rasa</t>
+  </si>
+  <si>
+    <t>Komal Dha</t>
+  </si>
+  <si>
+    <t>Komal Ga</t>
+  </si>
+  <si>
+    <t>Komal Re</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Komal Ga </t>
+  </si>
+  <si>
+    <t>Komal Ni</t>
   </si>
 </sst>
 </file>
@@ -588,12 +606,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -608,8 +632,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -935,18 +961,18 @@
     <col min="1" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" customWidth="1"/>
+    <col min="6" max="7" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -958,18 +984,21 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -980,13 +1009,16 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -998,15 +1030,18 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -1021,15 +1056,18 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -1041,38 +1079,44 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>181</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -1083,13 +1127,16 @@
       <c r="F7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -1100,13 +1147,16 @@
       <c r="F8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1117,36 +1167,42 @@
       <c r="F9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>182</v>
       </c>
       <c r="F10" t="s">
         <v>18</v>
       </c>
       <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
@@ -1161,35 +1217,41 @@
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -1201,32 +1263,38 @@
         <v>21</v>
       </c>
       <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
@@ -1238,72 +1306,84 @@
         <v>11</v>
       </c>
       <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
         <v>18</v>
       </c>
-      <c r="H15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>182</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D17" t="s">
         <v>34</v>
       </c>
       <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="F17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" t="s">
+        <v>181</v>
+      </c>
+      <c r="F18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
-        <v>141</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
@@ -1314,13 +1394,16 @@
       <c r="F19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -1331,13 +1414,16 @@
       <c r="F20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
@@ -1348,13 +1434,16 @@
       <c r="F21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
@@ -1366,66 +1455,78 @@
         <v>21</v>
       </c>
       <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" t="s">
         <v>9</v>
-      </c>
-      <c r="E23" t="s">
-        <v>25</v>
       </c>
       <c r="F23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>183</v>
       </c>
       <c r="E25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F25" t="s">
         <v>45</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
       <c r="B26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1439,13 +1540,16 @@
       <c r="G26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -1456,13 +1560,16 @@
       <c r="F27" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D28" t="s">
         <v>34</v>
@@ -1473,50 +1580,59 @@
       <c r="F28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" t="s">
         <v>50</v>
       </c>
-      <c r="B29" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B30" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>52</v>
       </c>
-      <c r="B30" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>53</v>
-      </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
@@ -1528,15 +1644,18 @@
         <v>11</v>
       </c>
       <c r="G31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -1547,16 +1666,19 @@
       <c r="F32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" t="s">
         <v>55</v>
-      </c>
-      <c r="B33" t="s">
-        <v>144</v>
-      </c>
-      <c r="D33" t="s">
-        <v>56</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
@@ -1567,13 +1689,16 @@
       <c r="G33" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -1585,15 +1710,18 @@
         <v>10</v>
       </c>
       <c r="G34" t="s">
+        <v>36</v>
+      </c>
+      <c r="H34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D35" t="s">
         <v>25</v>
@@ -1602,15 +1730,18 @@
         <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="G35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C36" t="s">
         <v>19</v>
@@ -1627,19 +1758,22 @@
       <c r="G36" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D37" t="s">
         <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F37" t="s">
         <v>21</v>
@@ -1647,33 +1781,39 @@
       <c r="G37" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>61</v>
       </c>
-      <c r="B38" t="s">
-        <v>138</v>
-      </c>
-      <c r="D38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E38" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" t="s">
-        <v>21</v>
-      </c>
-      <c r="G38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>62</v>
-      </c>
       <c r="B39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
@@ -1685,15 +1825,18 @@
         <v>11</v>
       </c>
       <c r="G39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
@@ -1704,13 +1847,16 @@
       <c r="F40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -1722,18 +1868,21 @@
         <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="H41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -1742,32 +1891,38 @@
         <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="H42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D43" t="s">
         <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F43" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
@@ -1779,15 +1934,18 @@
         <v>21</v>
       </c>
       <c r="G44" t="s">
+        <v>36</v>
+      </c>
+      <c r="H44" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -1799,15 +1957,18 @@
         <v>11</v>
       </c>
       <c r="G45" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
@@ -1818,13 +1979,16 @@
       <c r="F46" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C47" t="s">
         <v>27</v>
@@ -1836,52 +2000,61 @@
         <v>5</v>
       </c>
       <c r="F47" t="s">
+        <v>70</v>
+      </c>
+      <c r="G47" t="s">
+        <v>70</v>
+      </c>
+      <c r="H47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>71</v>
       </c>
-      <c r="G47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>72</v>
-      </c>
       <c r="B48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D48" t="s">
         <v>34</v>
       </c>
       <c r="E48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F48" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D49" t="s">
         <v>34</v>
       </c>
       <c r="E49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F49" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D50" t="s">
         <v>15</v>
@@ -1890,35 +2063,41 @@
         <v>25</v>
       </c>
       <c r="F50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G50" t="s">
+        <v>36</v>
+      </c>
+      <c r="H50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" t="s">
+        <v>175</v>
+      </c>
+      <c r="D51" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>75</v>
       </c>
-      <c r="B51" t="s">
-        <v>176</v>
-      </c>
-      <c r="D51" t="s">
-        <v>51</v>
-      </c>
-      <c r="E51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>76</v>
-      </c>
       <c r="B52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
@@ -1929,13 +2108,16 @@
       <c r="F52" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D53" t="s">
         <v>15</v>
@@ -1944,15 +2126,18 @@
         <v>16</v>
       </c>
       <c r="F53" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="G53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D54" t="s">
         <v>9</v>
@@ -1963,16 +2148,19 @@
       <c r="F54" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E55" t="s">
         <v>9</v>
@@ -1980,13 +2168,16 @@
       <c r="F55" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
@@ -1997,19 +2188,22 @@
       <c r="F56" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D57" t="s">
         <v>34</v>
       </c>
       <c r="E57" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F57" t="s">
         <v>21</v>
@@ -2017,13 +2211,16 @@
       <c r="G57" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D58" t="s">
         <v>34</v>
@@ -2032,15 +2229,18 @@
         <v>6</v>
       </c>
       <c r="F58" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="G58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B59" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
@@ -2049,21 +2249,24 @@
         <v>25</v>
       </c>
       <c r="F59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G59" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="H59" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E60" t="s">
         <v>9</v>
@@ -2072,32 +2275,38 @@
         <v>26</v>
       </c>
       <c r="G60" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="H60" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D61" t="s">
         <v>34</v>
       </c>
       <c r="E61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F61" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="G61" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D62" t="s">
         <v>6</v>
@@ -2108,13 +2317,16 @@
       <c r="F62" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
@@ -2123,15 +2335,18 @@
         <v>5</v>
       </c>
       <c r="F63" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="G63" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
@@ -2142,30 +2357,36 @@
       <c r="F64" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D65" t="s">
         <v>34</v>
       </c>
       <c r="E65" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F65" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="G65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D66" t="s">
         <v>25</v>
@@ -2174,15 +2395,18 @@
         <v>9</v>
       </c>
       <c r="F66" t="s">
+        <v>90</v>
+      </c>
+      <c r="G66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>92</v>
-      </c>
       <c r="B67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D67" t="s">
         <v>34</v>
@@ -2193,13 +2417,16 @@
       <c r="F67" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G67" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D68" t="s">
         <v>25</v>
@@ -2211,15 +2438,18 @@
         <v>21</v>
       </c>
       <c r="G68" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="H68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D69" t="s">
         <v>9</v>
@@ -2230,16 +2460,19 @@
       <c r="F69" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G69" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B70" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E70" t="s">
         <v>9</v>
@@ -2247,13 +2480,16 @@
       <c r="F70" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D71" t="s">
         <v>15</v>
@@ -2262,18 +2498,21 @@
         <v>16</v>
       </c>
       <c r="F71" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="G71" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E72" t="s">
         <v>5</v>
@@ -2281,13 +2520,16 @@
       <c r="F72" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G72" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B73" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D73" t="s">
         <v>25</v>
@@ -2296,44 +2538,54 @@
         <v>9</v>
       </c>
       <c r="F73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="G73" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D74" t="s">
         <v>34</v>
       </c>
       <c r="E74" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F74" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G74" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D75" t="s">
         <v>34</v>
       </c>
       <c r="E75" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F75" t="s">
         <v>21</v>
       </c>
+      <c r="G75" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I75" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add Stat tests pipeline
</commit_message>
<xml_diff>
--- a/RagaList.xlsx
+++ b/RagaList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhythmjain/GT-files/2-2/CompMus/ComputationalMusicology-TheRagaGuide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4A00FB-CC9E-5647-8017-5325E8ACF4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A19EF7-00C3-A84D-9519-7389D19B2ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$75</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="184">
   <si>
     <t>Raga</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Bihag</t>
   </si>
   <si>
-    <t xml:space="preserve">Ga </t>
-  </si>
-  <si>
     <t>Bilaskhani Todi</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Gorakh Kalyan</t>
   </si>
   <si>
-    <t xml:space="preserve">Ma </t>
-  </si>
-  <si>
     <t>Gujari Todi</t>
   </si>
   <si>
@@ -203,9 +197,6 @@
     <t>Hansadhvani</t>
   </si>
   <si>
-    <t xml:space="preserve">Sa </t>
-  </si>
-  <si>
     <t>Hindol</t>
   </si>
   <si>
@@ -591,6 +582,12 @@
   </si>
   <si>
     <t>Komal Ni</t>
+  </si>
+  <si>
+    <t>ALT_Rasa2</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -606,18 +603,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -632,9 +623,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -950,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -961,18 +951,18 @@
     <col min="1" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="7" width="27.33203125" customWidth="1"/>
+    <col min="6" max="8" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -984,21 +974,24 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H1" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="I1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="J1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1010,15 +1003,18 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -1033,15 +1029,18 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -1059,15 +1058,18 @@
         <v>11</v>
       </c>
       <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -1082,24 +1084,27 @@
         <v>17</v>
       </c>
       <c r="H5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -1107,16 +1112,19 @@
       <c r="G6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -1130,13 +1138,16 @@
       <c r="G7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -1150,13 +1161,16 @@
       <c r="G8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1170,22 +1184,25 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F10" t="s">
         <v>18</v>
@@ -1194,15 +1211,18 @@
         <v>11</v>
       </c>
       <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
@@ -1220,38 +1240,44 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="B12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -1266,35 +1292,41 @@
         <v>11</v>
       </c>
       <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
@@ -1309,27 +1341,30 @@
         <v>11</v>
       </c>
       <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
         <v>18</v>
       </c>
-      <c r="I15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
@@ -1337,53 +1372,62 @@
       <c r="G16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="G18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
@@ -1397,13 +1441,16 @@
       <c r="G19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -1417,13 +1464,16 @@
       <c r="G20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
@@ -1437,13 +1487,16 @@
       <c r="G21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
@@ -1458,15 +1511,18 @@
         <v>11</v>
       </c>
       <c r="H22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1478,15 +1534,18 @@
         <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
@@ -1500,33 +1559,39 @@
       <c r="G24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D25" t="s">
+        <v>180</v>
+      </c>
+      <c r="E25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" t="s">
         <v>183</v>
       </c>
-      <c r="E25" t="s">
-        <v>184</v>
-      </c>
-      <c r="F25" t="s">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>45</v>
       </c>
-      <c r="G25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>46</v>
-      </c>
       <c r="B26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1543,13 +1608,16 @@
       <c r="H26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -1563,16 +1631,19 @@
       <c r="G27" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
@@ -1583,79 +1654,91 @@
       <c r="G28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B30" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>50</v>
       </c>
-      <c r="E29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E31" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" t="s">
-        <v>122</v>
-      </c>
-      <c r="D31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>53</v>
-      </c>
       <c r="B32" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -1669,16 +1752,19 @@
       <c r="G32" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
@@ -1692,13 +1778,16 @@
       <c r="H33" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -1710,18 +1799,21 @@
         <v>10</v>
       </c>
       <c r="G34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H34" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D35" t="s">
         <v>25</v>
@@ -1730,50 +1822,56 @@
         <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C36" t="s">
         <v>19</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>177</v>
       </c>
       <c r="E36" t="s">
+        <v>178</v>
+      </c>
+      <c r="F36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" t="s">
         <v>16</v>
       </c>
-      <c r="F36" t="s">
-        <v>21</v>
-      </c>
-      <c r="G36" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" t="s">
-        <v>157</v>
-      </c>
-      <c r="D37" t="s">
-        <v>34</v>
-      </c>
       <c r="E37" t="s">
-        <v>44</v>
+        <v>181</v>
       </c>
       <c r="F37" t="s">
         <v>21</v>
@@ -1784,16 +1882,19 @@
       <c r="H37" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="E38" t="s">
         <v>5</v>
@@ -1802,18 +1903,21 @@
         <v>21</v>
       </c>
       <c r="G38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
@@ -1828,21 +1932,24 @@
         <v>11</v>
       </c>
       <c r="H39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="I39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F40" t="s">
         <v>21</v>
@@ -1850,19 +1957,22 @@
       <c r="G40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F41" t="s">
         <v>10</v>
@@ -1871,21 +1981,24 @@
         <v>10</v>
       </c>
       <c r="H41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+      <c r="I41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="s">
         <v>10</v>
@@ -1894,21 +2007,24 @@
         <v>10</v>
       </c>
       <c r="H42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+      <c r="I42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D43" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>44</v>
+        <v>181</v>
       </c>
       <c r="F43" t="s">
         <v>21</v>
@@ -1916,13 +2032,16 @@
       <c r="G43" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
@@ -1934,18 +2053,21 @@
         <v>21</v>
       </c>
       <c r="G44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H44" t="s">
+        <v>35</v>
+      </c>
+      <c r="I44" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B45" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -1960,15 +2082,18 @@
         <v>11</v>
       </c>
       <c r="H45" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="I45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
@@ -1982,13 +2107,16 @@
       <c r="G46" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C47" t="s">
         <v>27</v>
@@ -2000,107 +2128,122 @@
         <v>5</v>
       </c>
       <c r="F47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47" t="s">
+        <v>67</v>
+      </c>
+      <c r="H47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" t="s">
+        <v>156</v>
+      </c>
+      <c r="D48" t="s">
+        <v>180</v>
+      </c>
+      <c r="E48" t="s">
+        <v>181</v>
+      </c>
+      <c r="F48" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>70</v>
       </c>
-      <c r="G47" t="s">
-        <v>70</v>
-      </c>
-      <c r="H47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" t="s">
+        <v>179</v>
+      </c>
+      <c r="E50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" t="s">
+        <v>35</v>
+      </c>
+      <c r="G50" t="s">
+        <v>35</v>
+      </c>
+      <c r="H50" t="s">
+        <v>35</v>
+      </c>
+      <c r="I50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>71</v>
       </c>
-      <c r="B48" t="s">
-        <v>159</v>
-      </c>
-      <c r="D48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" t="s">
-        <v>21</v>
-      </c>
-      <c r="G48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="B51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" t="s">
+        <v>21</v>
+      </c>
+      <c r="H51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>72</v>
       </c>
-      <c r="B49" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" t="s">
-        <v>44</v>
-      </c>
-      <c r="F49" t="s">
-        <v>21</v>
-      </c>
-      <c r="G49" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" t="s">
-        <v>25</v>
-      </c>
-      <c r="F50" t="s">
-        <v>36</v>
-      </c>
-      <c r="G50" t="s">
-        <v>36</v>
-      </c>
-      <c r="H50" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" t="s">
-        <v>175</v>
-      </c>
-      <c r="D51" t="s">
-        <v>50</v>
-      </c>
-      <c r="E51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F51" t="s">
-        <v>21</v>
-      </c>
-      <c r="G51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>75</v>
-      </c>
       <c r="B52" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E52" t="s">
         <v>5</v>
@@ -2111,33 +2254,39 @@
       <c r="G52" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B53" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D53" t="s">
-        <v>15</v>
+        <v>177</v>
       </c>
       <c r="E53" t="s">
-        <v>16</v>
+        <v>178</v>
       </c>
       <c r="F53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G53" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D54" t="s">
         <v>9</v>
@@ -2151,19 +2300,22 @@
       <c r="G54" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D55" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F55" t="s">
         <v>21</v>
@@ -2171,13 +2323,16 @@
       <c r="G55" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B56" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
@@ -2189,21 +2344,24 @@
         <v>7</v>
       </c>
       <c r="G56" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D57" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F57" t="s">
         <v>21</v>
@@ -2214,59 +2372,68 @@
       <c r="H57" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D58" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E58" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="F58" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G58" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="H58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
       </c>
       <c r="E59" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F59" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G59" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H59" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B60" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D60" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="E60" t="s">
         <v>9</v>
@@ -2275,44 +2442,50 @@
         <v>26</v>
       </c>
       <c r="G60" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H60" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I60" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B61" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D61" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F61" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G61" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D62" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E62" t="s">
-        <v>5</v>
+        <v>181</v>
       </c>
       <c r="F62" t="s">
         <v>21</v>
@@ -2320,13 +2493,16 @@
       <c r="G62" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B63" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
@@ -2335,18 +2511,21 @@
         <v>5</v>
       </c>
       <c r="F63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G63" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
@@ -2360,56 +2539,65 @@
       <c r="G64" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H64" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B65" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D65" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E65" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G65" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="H65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B66" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D66" t="s">
-        <v>25</v>
+        <v>179</v>
       </c>
       <c r="E66" t="s">
         <v>9</v>
       </c>
       <c r="F66" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G66" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="H66" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B67" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D67" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E67" t="s">
         <v>15</v>
@@ -2420,13 +2608,16 @@
       <c r="G67" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H67" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D68" t="s">
         <v>25</v>
@@ -2438,18 +2629,21 @@
         <v>21</v>
       </c>
       <c r="G68" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H68" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D69" t="s">
         <v>9</v>
@@ -2463,16 +2657,19 @@
       <c r="G69" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H69" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D70" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="E70" t="s">
         <v>9</v>
@@ -2483,13 +2680,16 @@
       <c r="G70" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B71" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D71" t="s">
         <v>15</v>
@@ -2498,21 +2698,24 @@
         <v>16</v>
       </c>
       <c r="F71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G71" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H71" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B72" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D72" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="E72" t="s">
         <v>5</v>
@@ -2523,39 +2726,45 @@
       <c r="G72" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H72" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B73" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D73" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E73" t="s">
         <v>9</v>
       </c>
       <c r="F73" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G73" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="H73" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B74" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D74" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E74" t="s">
-        <v>44</v>
+        <v>181</v>
       </c>
       <c r="F74" t="s">
         <v>21</v>
@@ -2563,19 +2772,22 @@
       <c r="G74" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>99</v>
+      <c r="H74" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="B75" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D75" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E75" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F75" t="s">
         <v>21</v>
@@ -2583,9 +2795,12 @@
       <c r="G75" t="s">
         <v>21</v>
       </c>
+      <c r="H75" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I75" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J75" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>